<commit_message>
refactor_ Lógica implementada para validar proyectos en transición de asignación de ejecutivo técnico (PD)
</commit_message>
<xml_diff>
--- a/Proyectos a distribuir cartera PD.xlsx
+++ b/Proyectos a distribuir cartera PD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://corfocl.sharepoint.com/sites/UNIDADDECONTROLYGESTINDEPROCESOS/Documentos compartidos/Configuraciones y Reconfiguraciones/Reportería reconfiguraciones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4950483-8833-485A-ACD1-D6B59363698B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{C4950483-8833-485A-ACD1-D6B59363698B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF8C5B0C-3E58-41E5-90F6-458F8160418D}"/>
   <bookViews>
     <workbookView xWindow="-17880" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{4ABFA1F5-DE0B-41B8-A10C-E466E3B974D9}"/>
   </bookViews>
@@ -2226,10 +2226,10 @@
   <dimension ref="A1:AA40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22:C40"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5373,7 +5373,7 @@
   <autoFilter ref="A1:AA40" xr:uid="{F405D811-0458-425C-9356-0382DD02C671}">
     <filterColumn colId="2">
       <filters>
-        <filter val="PABLO GAETE"/>
+        <filter val="PABLO GAETE HALLER"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5382,6 +5382,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3abb5c61-2b1c-49a7-ae5a-ca2e205864ad">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="21d2f484-8766-420c-be76-4087dc036e0d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010094B6624CBDBCCF47BCB8BFE999D45502" ma:contentTypeVersion="14" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="2c7f2b64bc6c41c1b3e41751aed88bed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3abb5c61-2b1c-49a7-ae5a-ca2e205864ad" xmlns:ns3="21d2f484-8766-420c-be76-4087dc036e0d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6344dba601b4f5a55cb8cee6aa41064d" ns2:_="" ns3:_="">
     <xsd:import namespace="3abb5c61-2b1c-49a7-ae5a-ca2e205864ad"/>
@@ -5610,34 +5630,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3abb5c61-2b1c-49a7-ae5a-ca2e205864ad">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="21d2f484-8766-420c-be76-4087dc036e0d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05F50E84-7468-4E87-BC42-02D050FBAA1A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FB259D6-D8D1-4C6C-9C66-D02876E65682}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3abb5c61-2b1c-49a7-ae5a-ca2e205864ad"/>
+    <ds:schemaRef ds:uri="21d2f484-8766-420c-be76-4087dc036e0d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24A39E70-7820-4C32-9BA1-7381DFEB1D2D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24A39E70-7820-4C32-9BA1-7381DFEB1D2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FB259D6-D8D1-4C6C-9C66-D02876E65682}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05F50E84-7468-4E87-BC42-02D050FBAA1A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3abb5c61-2b1c-49a7-ae5a-ca2e205864ad"/>
+    <ds:schemaRef ds:uri="21d2f484-8766-420c-be76-4087dc036e0d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>